<commit_message>
Updated the DAX query file
</commit_message>
<xml_diff>
--- a/DAX_query_refrences.xlsx
+++ b/DAX_query_refrences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Projects\PWC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Projects\Power-BI-for-interviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2470F100-2AE1-4706-83A3-881A845F0E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3CCAFFD4-DEC0-4614-B496-54F6E83749F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,8 +293,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,12 +337,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.14999847407452621"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -741,11 +735,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,163 +756,163 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
         <v>41</v>
       </c>
+      <c r="B11" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B12" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="96.6" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="69" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="69" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>